<commit_message>
Build After First Run.
</commit_message>
<xml_diff>
--- a/TestOutput/Inputs.xlsx
+++ b/TestOutput/Inputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
   <si>
     <t>tc_id</t>
   </si>
@@ -218,7 +218,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="49">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +236,258 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="63"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
       <b val="true"/>
     </font>
     <font>
@@ -289,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -298,6 +550,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -642,7 +936,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" t="s" s="37">
         <v>64</v>
       </c>
     </row>
@@ -655,6 +949,9 @@
       </c>
       <c r="C4" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" t="s" s="49">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -755,6 +1052,9 @@
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4" t="s" s="8">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="5" spans="1:6">
       <c r="A5" t="s">
@@ -772,6 +1072,9 @@
       <c r="E5" t="s">
         <v>40</v>
       </c>
+      <c r="F5" t="s" s="10">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="6" spans="1:6">
       <c r="A6" t="s">
@@ -789,6 +1092,9 @@
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6" t="s" s="12">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="7" spans="1:6">
       <c r="A7" t="s">
@@ -806,6 +1112,9 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
+      <c r="F7" t="s" s="14">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="8" spans="1:6">
       <c r="A8" t="s">
@@ -823,6 +1132,9 @@
       <c r="E8">
         <v>10</v>
       </c>
+      <c r="F8" t="s" s="16">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="9" spans="1:6">
       <c r="A9" t="s">
@@ -840,6 +1152,9 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
+      <c r="F9" t="s" s="18">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="10" spans="1:6">
       <c r="A10" t="s">
@@ -857,6 +1172,9 @@
       <c r="E10">
         <v>10</v>
       </c>
+      <c r="F10" t="s" s="20">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="11" spans="1:6">
       <c r="A11" t="s">
@@ -874,6 +1192,9 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
+      <c r="F11" t="s" s="22">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="12" spans="1:6">
       <c r="A12" t="s">
@@ -891,6 +1212,9 @@
       <c r="E12">
         <v>10</v>
       </c>
+      <c r="F12" t="s" s="24">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="13" spans="1:6">
       <c r="A13" t="s">
@@ -908,6 +1232,9 @@
       <c r="E13" t="s">
         <v>16</v>
       </c>
+      <c r="F13" t="s" s="26">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="14" spans="1:6">
       <c r="A14" t="s">
@@ -925,6 +1252,9 @@
       <c r="E14">
         <v>10</v>
       </c>
+      <c r="F14" t="s" s="28">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="15" spans="1:6">
       <c r="A15" t="s">
@@ -942,6 +1272,9 @@
       <c r="E15" t="s">
         <v>16</v>
       </c>
+      <c r="F15" t="s" s="30">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="16" spans="1:6">
       <c r="A16" t="s">
@@ -959,6 +1292,9 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
+      <c r="F16" t="s" s="32">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="17" spans="1:5">
       <c r="A17" t="s">
@@ -976,6 +1312,9 @@
       <c r="E17">
         <v>20</v>
       </c>
+      <c r="F17" t="s" s="34">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="24.75" r="18" spans="1:5">
       <c r="A18" t="s">
@@ -992,6 +1331,9 @@
       </c>
       <c r="E18" t="s">
         <v>16</v>
+      </c>
+      <c r="F18" t="s" s="36">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1049,6 +1391,9 @@
       <c r="E2">
         <v>10</v>
       </c>
+      <c r="F2" t="s" s="38">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="3" spans="1:6">
       <c r="A3" t="s">
@@ -1066,6 +1411,9 @@
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3" t="s" s="40">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="4" spans="1:6">
       <c r="A4" t="s">
@@ -1083,6 +1431,9 @@
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4" t="s" s="42">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="5" spans="1:6">
       <c r="A5" t="s">
@@ -1100,6 +1451,9 @@
       <c r="E5">
         <v>3</v>
       </c>
+      <c r="F5" t="s" s="44">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="6" spans="1:6">
       <c r="A6" t="s">
@@ -1117,6 +1471,9 @@
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6" t="s" s="46">
+        <v>64</v>
+      </c>
     </row>
     <row customHeight="1" ht="19.5" r="7" spans="1:6">
       <c r="A7" t="s">
@@ -1133,6 +1490,9 @@
       </c>
       <c r="E7" t="s">
         <v>16</v>
+      </c>
+      <c r="F7" t="s" s="48">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>